<commit_message>
11 July - 6.25
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prashanth.venkatesan\Documents\Efile\RE_Efile_IT_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449FB14F-ECCA-4F7D-93B9-73BBDB2D37F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F285A6EA-E758-4112-8742-BAABB0D146E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,9 +87,6 @@
     <t>logF_BusinessProcessName</t>
   </si>
   <si>
-    <t>Framework</t>
-  </si>
-  <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>C:\Users\%USERID%\AppData\Local\Programs\ITDe-Filing-2023\ITDe-Filing-2023.exe</t>
+  </si>
+  <si>
+    <t>RE_Efile_IT_Performer</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -609,22 +609,22 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -633,44 +633,44 @@
         <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1725,18 +1725,18 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1760,7 +1760,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1782,7 +1782,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1793,7 +1793,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1804,53 +1804,53 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" t="b">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2854,7 +2854,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2884,18 +2884,18 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>